<commit_message>
update script for automation
</commit_message>
<xml_diff>
--- a/data_manipulation/weather/weather_dialogue.xlsx
+++ b/data_manipulation/weather/weather_dialogue.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhengyitang/Tunnel/Github Repo/tunnel_transit/data_manipulation/weather/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCF3BFF1-BC0D-5B44-ABC8-8E480158D9EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C291413-0AEE-F347-836F-24883A26AA92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2240" yWindow="1120" windowWidth="52280" windowHeight="27100" xr2:uid="{85B6EFB7-C658-E74B-944E-2EE3918E122D}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>hot1</t>
   </si>
@@ -490,9 +490,6 @@
   </si>
   <si>
     <t>听说有些人发明了能抵御紫外线的东西。不如试试看？</t>
-  </si>
-  <si>
-    <t>7, 5</t>
   </si>
 </sst>
 </file>
@@ -850,10 +847,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A070831-4A46-934A-B3AF-943A355635A4}">
-  <dimension ref="A1:BX3"/>
+  <dimension ref="A1:BX2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="141" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1395,11 +1392,6 @@
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:76" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
-        <v>152</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>